<commit_message>
Atualização - RDD 13 e Copas
Atualização das pontuações da Rodada 13 e também ajustes da Fase 3 da Libertadores
</commit_message>
<xml_diff>
--- a/liga_eliminacao/datasets_liga_eliminacao/Pontuacoes_Por_Rodada_Liga_Eliminacao.xlsx
+++ b/liga_eliminacao/datasets_liga_eliminacao/Pontuacoes_Por_Rodada_Liga_Eliminacao.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Rodada 1</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Rodada 12</t>
+  </si>
+  <si>
+    <t>Rodada 13</t>
   </si>
   <si>
     <t>KING LEONN</t>
@@ -503,13 +506,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -546,10 +549,13 @@
       <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>79.2998046875</v>
@@ -582,9 +588,9 @@
         <v>40.77001953125</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>77.580078125</v>
@@ -622,10 +628,13 @@
       <c r="M3">
         <v>56.260009765625</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="N3">
+        <v>107.64990234375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>64.08984375</v>
@@ -663,10 +672,13 @@
       <c r="M4">
         <v>62.260009765625</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="N4">
+        <v>96.509765625</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>96.18994140625</v>
@@ -704,10 +716,13 @@
       <c r="M5">
         <v>56.4599609375</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="N5">
+        <v>70.2099609375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>72.58984375</v>
@@ -745,10 +760,13 @@
       <c r="M6">
         <v>69.91015625</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="N6">
+        <v>118.740234375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>95.22998046875</v>
@@ -781,9 +799,9 @@
         <v>53.3701171875</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8">
         <v>75.330078125</v>
@@ -821,10 +839,13 @@
       <c r="M8">
         <v>44.77001953125</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="N8">
+        <v>110.41015625</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9">
         <v>67.990234375</v>
@@ -862,10 +883,13 @@
       <c r="M9">
         <v>66.9599609375</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="N9">
+        <v>117.509765625</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10">
         <v>84.68994140625</v>
@@ -903,18 +927,21 @@
       <c r="M10">
         <v>58.840087890625</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="N10">
+        <v>128.0400390625</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11">
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12">
         <v>60.550048828125</v>
@@ -952,10 +979,13 @@
       <c r="M12">
         <v>62.760009765625</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="N12">
+        <v>93.509765625</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B13">
         <v>67.68994140625</v>
@@ -993,10 +1023,13 @@
       <c r="M13">
         <v>69.259765625</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="N13">
+        <v>111.91015625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B14">
         <v>72.3798828125</v>
@@ -1034,10 +1067,13 @@
       <c r="M14">
         <v>65.81005859375</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="N14">
+        <v>117.10986328125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B15">
         <v>61.550048828125</v>
@@ -1075,10 +1111,13 @@
       <c r="M15">
         <v>65.85986328125</v>
       </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="N15">
+        <v>133.0498046875</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B16">
         <v>63.5</v>
@@ -1087,9 +1126,9 @@
         <v>46.919921875</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:14">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B17">
         <v>73.77978515625</v>
@@ -1125,9 +1164,9 @@
         <v>72.16015625</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:14">
       <c r="A18" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B18">
         <v>68.39990234375</v>
@@ -1139,9 +1178,9 @@
         <v>38.219970703125</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:14">
       <c r="A19" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B19">
         <v>64.7900390625</v>
@@ -1179,10 +1218,13 @@
       <c r="M19">
         <v>55.760009765625</v>
       </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="N19">
+        <v>113.509765625</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B20">
         <v>63.64990234375</v>
@@ -1221,9 +1263,9 @@
         <v>40.739990234375</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:14">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B21">
         <v>66.60009765625</v>
@@ -1261,10 +1303,13 @@
       <c r="M21">
         <v>50.10009765625</v>
       </c>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="N21">
+        <v>79.41015625</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B22">
         <v>74.08984375</v>
@@ -1302,10 +1347,13 @@
       <c r="M22">
         <v>59.47998046875</v>
       </c>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="N22">
+        <v>120.8701171875</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B23">
         <v>67.14013671875</v>
@@ -1323,9 +1371,9 @@
         <v>59.919921875</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:14">
       <c r="A24" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B24">
         <v>72.2900390625</v>
@@ -1346,9 +1394,9 @@
         <v>48.840087890625</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:14">
       <c r="A25" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B25">
         <v>69.4501953125</v>
@@ -1378,9 +1426,9 @@
         <v>56.8701171875</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:14">
       <c r="A26" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B26">
         <v>66.5</v>
@@ -1418,10 +1466,13 @@
       <c r="M26">
         <v>67.31005859375</v>
       </c>
-    </row>
-    <row r="27" spans="1:13">
+      <c r="N26">
+        <v>119.41015625</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B27">
         <v>61.14990234375</v>
@@ -1436,9 +1487,9 @@
         <v>51.6298828125</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:14">
       <c r="A28" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B28">
         <v>68.47998046875</v>
@@ -1465,9 +1516,9 @@
         <v>46.89990234375</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:14">
       <c r="A29" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B29">
         <v>100.33984375</v>
@@ -1506,9 +1557,9 @@
         <v>44.4599609375</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:14">
       <c r="A30" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B30">
         <v>72.240234375</v>
@@ -1544,9 +1595,9 @@
         <v>69.14990234375</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:14">
       <c r="A31" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B31">
         <v>82.68017578125</v>
@@ -1570,9 +1621,9 @@
         <v>79.7001953125</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:14">
       <c r="A32" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B32">
         <v>77.0498046875</v>
@@ -1610,10 +1661,13 @@
       <c r="M32">
         <v>75.85986328125</v>
       </c>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="N32">
+        <v>124.31005859375</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B33">
         <v>64</v>
@@ -1650,6 +1704,9 @@
       </c>
       <c r="M33">
         <v>95.66015625</v>
+      </c>
+      <c r="N33">
+        <v>130.2099609375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>